<commit_message>
refactor code and change method API by RestFull
</commit_message>
<xml_diff>
--- a/Book App Store.xlsx
+++ b/Book App Store.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\NashTech\book_store_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543394BB-1384-4EA6-8D80-9D186D91E411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A140A941-6BAC-45A4-8DB1-567D595509D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{545E2824-613D-478B-A8F8-50EDAE3FA5C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12456" xr2:uid="{545E2824-613D-478B-A8F8-50EDAE3FA5C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>Book Store App</t>
   </si>
@@ -144,6 +144,42 @@
   </si>
   <si>
     <t>DashboardController</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>api/v1/books</t>
+  </si>
+  <si>
+    <t>api/v1/books/{bookId}</t>
+  </si>
+  <si>
+    <t>api/v1/books/{bookId}/restore</t>
+  </si>
+  <si>
+    <t>api/v1/books/{bookId}/views</t>
+  </si>
+  <si>
+    <t>!is_admin</t>
+  </si>
+  <si>
+    <t>is_admin</t>
+  </si>
+  <si>
+    <t>api/v1/get-user-login</t>
   </si>
 </sst>
 </file>
@@ -183,7 +219,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -268,23 +304,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -292,33 +389,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -635,197 +711,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464C2728-8F58-4023-AB09-4B070B4DB5BA}">
-  <dimension ref="A2:K29"/>
+  <dimension ref="A2:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="10" width="9.21875" customWidth="1"/>
     <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="3" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="F6" s="16"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>3</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="4" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
         <v>4</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="7" t="s">
+      <c r="F9" s="16"/>
+      <c r="G9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6" t="s">
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8" t="s">
+      <c r="F10" s="16"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="F11" s="16"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="17"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -838,334 +915,386 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11" t="s">
+      <c r="F16" s="15"/>
+      <c r="G16" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="3" t="s">
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+      <c r="L16" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="12" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="9" t="s">
+      <c r="F17" s="8"/>
+      <c r="G17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>2</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="9" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>3</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="9" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="4" t="s">
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="9" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="4" t="s">
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="O20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="G21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="20">
+        <v>6</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="9" t="s">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
-        <v>6</v>
-      </c>
-      <c r="B22" s="9" t="s">
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="M22" t="s">
+        <v>46</v>
+      </c>
+      <c r="O22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="21"/>
+      <c r="B23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L23" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" t="s">
+        <v>47</v>
+      </c>
+      <c r="O23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>7</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="9" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="O24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>8</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="O25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>9</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="9" t="s">
+      <c r="L26" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>10</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
-        <v>8</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="4" t="s">
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
-        <v>9</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="9" t="s">
+      <c r="L27" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="O27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>11</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="4" t="s">
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
-        <v>10</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="9" t="s">
+      <c r="L28" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="O28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>12</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="4" t="s">
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
-        <v>11</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
-        <v>12</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
-        <v>13</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="4" t="s">
-        <v>7</v>
+      <c r="L29" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="O29" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="E17:F20"/>
-    <mergeCell ref="E21:F23"/>
-    <mergeCell ref="E25:F29"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="E22:F29"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="G24:J24"/>
     <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:D11"/>
+    <mergeCell ref="G9:J11"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="B4:D4"/>
@@ -1176,19 +1305,38 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:D11"/>
-    <mergeCell ref="G9:J11"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="E11:F11"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:D6"/>
     <mergeCell ref="G5:J6"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E10:F10"/>
     <mergeCell ref="G7:J7"/>
     <mergeCell ref="G8:J8"/>
-    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="E17:F20"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="G21:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>